<commit_message>
Take out building tags for education/health; tagging points, leads to confusion
</commit_message>
<xml_diff>
--- a/OpenMapKit/hot_11_health.xlsx
+++ b/OpenMapKit/hot_11_health.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
   <si>
     <t>type</t>
   </si>
@@ -101,18 +101,6 @@
     <t>Opening hours</t>
   </si>
   <si>
-    <t>building:levels </t>
-  </si>
-  <si>
-    <t>Building levels (1, 2, 3, etc)</t>
-  </si>
-  <si>
-    <t>building:material </t>
-  </si>
-  <si>
-    <t>Building material</t>
-  </si>
-  <si>
     <t>bed_count</t>
   </si>
   <si>
@@ -164,51 +152,6 @@
     <t>Hospital (20+ people)</t>
   </si>
   <si>
-    <t>building:material</t>
-  </si>
-  <si>
-    <t>brick</t>
-  </si>
-  <si>
-    <t>Brick</t>
-  </si>
-  <si>
-    <t>cement_block</t>
-  </si>
-  <si>
-    <t>Cement blocks</t>
-  </si>
-  <si>
-    <t>concrete</t>
-  </si>
-  <si>
-    <t>Concrete (poured)</t>
-  </si>
-  <si>
-    <t>loam</t>
-  </si>
-  <si>
-    <t>Loam (branches+mud)</t>
-  </si>
-  <si>
-    <t>metal</t>
-  </si>
-  <si>
-    <t>Metal</t>
-  </si>
-  <si>
-    <t>plaster</t>
-  </si>
-  <si>
-    <t>Plaster</t>
-  </si>
-  <si>
-    <t>wood </t>
-  </si>
-  <si>
-    <t>Wood</t>
-  </si>
-  <si>
     <t>kampala</t>
   </si>
   <si>
@@ -248,10 +191,10 @@
     <t>Mo-Fr 08:00-18:00; Sa-Su 08:00-15:00</t>
   </si>
   <si>
+    <t>Iganga</t>
+  </si>
+  <si>
     <t>Jinja</t>
-  </si>
-  <si>
-    <t>Iganga</t>
   </si>
   <si>
     <t>form_id</t>
@@ -273,7 +216,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -305,19 +248,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -365,7 +295,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -394,15 +324,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -425,8 +347,8 @@
   </sheetPr>
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1722,6 +1644,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7040816326531"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.5714285714286"/>
     <col collapsed="false" hidden="false" max="26" min="7" style="0" width="8.70918367346939"/>
@@ -1778,10 +1701,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z58"/>
+  <dimension ref="A1:Z65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1931,13 +1854,13 @@
       <c r="Z4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="4"/>
@@ -2005,7 +1928,7 @@
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="4"/>
@@ -2073,7 +1996,7 @@
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="4"/>
@@ -2101,13 +2024,13 @@
       <c r="Z9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="4"/>
@@ -2135,15 +2058,9 @@
       <c r="Z10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -2169,15 +2086,9 @@
       <c r="Z11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -2203,9 +2114,15 @@
       <c r="Z12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -2260,13 +2177,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -2293,9 +2210,15 @@
       <c r="Z15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -2325,10 +2248,10 @@
         <v>21</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -2355,15 +2278,9 @@
       <c r="Z17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -2388,15 +2305,15 @@
       <c r="Y18" s="4"/>
       <c r="Z18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>47</v>
+    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -2422,10 +2339,16 @@
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -2450,15 +2373,15 @@
       <c r="Y20" s="4"/>
       <c r="Z20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -2484,16 +2407,10 @@
       <c r="Y21" s="4"/>
       <c r="Z21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>52</v>
-      </c>
+    <row r="22" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -2519,14 +2436,14 @@
       <c r="Z22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>54</v>
+      <c r="A23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -2552,15 +2469,15 @@
       <c r="Y23" s="4"/>
       <c r="Z23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>56</v>
+    <row r="24" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -2586,15 +2503,15 @@
       <c r="Y24" s="4"/>
       <c r="Z24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>58</v>
+    <row r="25" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -2620,15 +2537,15 @@
       <c r="Y25" s="4"/>
       <c r="Z25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>60</v>
+    <row r="26" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -2654,15 +2571,15 @@
       <c r="Y26" s="4"/>
       <c r="Z26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>62</v>
+    <row r="27" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -2689,9 +2606,15 @@
       <c r="Z27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="A28" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -2717,14 +2640,14 @@
       <c r="Z28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>64</v>
+      <c r="A29" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -2751,15 +2674,9 @@
       <c r="Z29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2785,14 +2702,14 @@
       <c r="Z30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>68</v>
+      <c r="A31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2819,9 +2736,15 @@
       <c r="Z31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="A32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -2846,15 +2769,15 @@
       <c r="Y32" s="4"/>
       <c r="Z32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>69</v>
+    <row r="33" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -2881,14 +2804,14 @@
       <c r="Z33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>70</v>
+      <c r="A34" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -2915,14 +2838,14 @@
       <c r="Z34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="s">
-        <v>25</v>
+      <c r="A35" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -2948,350 +2871,26 @@
       <c r="Y35" s="4"/>
       <c r="Z35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
-      <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
-      <c r="Z36" s="4"/>
-    </row>
-    <row r="37" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4"/>
-    </row>
-    <row r="38" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
-      <c r="S38" s="4"/>
-      <c r="T38" s="4"/>
-      <c r="U38" s="4"/>
-      <c r="V38" s="4"/>
-      <c r="W38" s="4"/>
-      <c r="X38" s="4"/>
-      <c r="Y38" s="4"/>
-      <c r="Z38" s="4"/>
-    </row>
-    <row r="39" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
-      <c r="T39" s="4"/>
-      <c r="U39" s="4"/>
-      <c r="V39" s="4"/>
-      <c r="W39" s="4"/>
-      <c r="X39" s="4"/>
-      <c r="Y39" s="4"/>
-      <c r="Z39" s="4"/>
-    </row>
-    <row r="40" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-      <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4"/>
-      <c r="S40" s="4"/>
-      <c r="T40" s="4"/>
-      <c r="U40" s="4"/>
-      <c r="V40" s="4"/>
-      <c r="W40" s="4"/>
-      <c r="X40" s="4"/>
-      <c r="Y40" s="4"/>
-      <c r="Z40" s="4"/>
-    </row>
-    <row r="41" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
-      <c r="S41" s="4"/>
-      <c r="T41" s="4"/>
-      <c r="U41" s="4"/>
-      <c r="V41" s="4"/>
-      <c r="W41" s="4"/>
-      <c r="X41" s="4"/>
-      <c r="Y41" s="4"/>
-      <c r="Z41" s="4"/>
-    </row>
-    <row r="42" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-      <c r="P42" s="4"/>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4"/>
-      <c r="S42" s="4"/>
-      <c r="T42" s="4"/>
-      <c r="U42" s="4"/>
-      <c r="V42" s="4"/>
-      <c r="W42" s="4"/>
-      <c r="X42" s="4"/>
-      <c r="Y42" s="4"/>
-      <c r="Z42" s="4"/>
-    </row>
-    <row r="43" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-      <c r="Q43" s="4"/>
-      <c r="R43" s="4"/>
-      <c r="S43" s="4"/>
-      <c r="T43" s="4"/>
-      <c r="U43" s="4"/>
-      <c r="V43" s="4"/>
-      <c r="W43" s="4"/>
-      <c r="X43" s="4"/>
-      <c r="Y43" s="4"/>
-      <c r="Z43" s="4"/>
-    </row>
-    <row r="44" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
-      <c r="T44" s="4"/>
-      <c r="U44" s="4"/>
-      <c r="V44" s="4"/>
-      <c r="W44" s="4"/>
-      <c r="X44" s="4"/>
-      <c r="Y44" s="4"/>
-      <c r="Z44" s="4"/>
-    </row>
-    <row r="45" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-      <c r="Q45" s="4"/>
-      <c r="R45" s="4"/>
-      <c r="S45" s="4"/>
-      <c r="T45" s="4"/>
-      <c r="U45" s="4"/>
-      <c r="V45" s="4"/>
-      <c r="W45" s="4"/>
-      <c r="X45" s="4"/>
-      <c r="Y45" s="4"/>
-      <c r="Z45" s="4"/>
-    </row>
-    <row r="48" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4228,15 +3827,14 @@
     <row r="991" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="992" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="993" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="994" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="995" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="996" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="997" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1001" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1002" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4270,10 +3868,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -4302,10 +3900,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>

</xml_diff>

<commit_message>
Oops, forgot main building tag. Again.
</commit_message>
<xml_diff>
--- a/OpenMapKit/hot_11_health.xlsx
+++ b/OpenMapKit/hot_11_health.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
   <si>
     <t>type</t>
   </si>
@@ -77,12 +77,6 @@
     <t>health_tags</t>
   </si>
   <si>
-    <t>building</t>
-  </si>
-  <si>
-    <t>Building (required)</t>
-  </si>
-  <si>
     <t>amenity</t>
   </si>
   <si>
@@ -131,22 +125,19 @@
     <t>Comments</t>
   </si>
   <si>
+    <t>doctors</t>
+  </si>
+  <si>
+    <t>Doctors (1-10 people)</t>
+  </si>
+  <si>
+    <t>clinic</t>
+  </si>
+  <si>
+    <t>Clinic (10-20 people)</t>
+  </si>
+  <si>
     <t>hospital</t>
-  </si>
-  <si>
-    <t>Hospital</t>
-  </si>
-  <si>
-    <t>doctors</t>
-  </si>
-  <si>
-    <t>Doctors (1-10 people)</t>
-  </si>
-  <si>
-    <t>clinic</t>
-  </si>
-  <si>
-    <t>Clinic (10-20 people)</t>
   </si>
   <si>
     <t>Hospital (20+ people)</t>
@@ -1704,7 +1695,7 @@
   <dimension ref="A1:Z65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1790,10 +1781,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -1820,14 +1811,14 @@
       <c r="Z3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>1</v>
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1854,13 +1845,13 @@
       <c r="Z4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="4"/>
@@ -1894,7 +1885,7 @@
       <c r="B6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="4"/>
@@ -1928,7 +1919,7 @@
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="4"/>
@@ -1990,13 +1981,13 @@
       <c r="Z8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="4"/>
@@ -2024,15 +2015,9 @@
       <c r="Z9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -2086,9 +2071,15 @@
       <c r="Z11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -2120,7 +2111,7 @@
       <c r="B13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="4"/>
@@ -2148,9 +2139,15 @@
       <c r="Z13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -2176,15 +2173,9 @@
       <c r="Z14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -2209,14 +2200,14 @@
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="4" t="s">
+    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="4"/>
@@ -2243,15 +2234,15 @@
       <c r="Y16" s="4"/>
       <c r="Z16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="6" t="s">
+    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>43</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -2277,10 +2268,16 @@
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -2306,15 +2303,9 @@
       <c r="Z18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -2339,12 +2330,12 @@
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>29</v>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>47</v>
@@ -2374,14 +2365,14 @@
       <c r="Z20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="7" t="s">
+      <c r="A21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>49</v>
+      <c r="C21" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -2408,9 +2399,15 @@
       <c r="Z21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -2435,14 +2432,14 @@
       <c r="Y22" s="4"/>
       <c r="Z22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D23" s="4"/>
@@ -2471,7 +2468,7 @@
     </row>
     <row r="24" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>51</v>
@@ -2505,7 +2502,7 @@
     </row>
     <row r="25" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>52</v>
@@ -2539,12 +2536,12 @@
     </row>
     <row r="26" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="7" t="s">
         <v>53</v>
       </c>
       <c r="D26" s="4"/>
@@ -2572,15 +2569,9 @@
       <c r="Z26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>54</v>
-      </c>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -2606,14 +2597,14 @@
       <c r="Z27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>55</v>
+      <c r="A28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -2640,14 +2631,14 @@
       <c r="Z28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
-        <v>25</v>
+      <c r="A29" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -2674,9 +2665,15 @@
       <c r="Z29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="A30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2702,14 +2699,14 @@
       <c r="Z30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>45</v>
+      <c r="A31" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2736,14 +2733,14 @@
       <c r="Z31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>29</v>
+      <c r="A32" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -2769,119 +2766,20 @@
       <c r="Y32" s="4"/>
       <c r="Z32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-      <c r="Z33" s="4"/>
-    </row>
-    <row r="34" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-      <c r="Z34" s="4"/>
-    </row>
-    <row r="35" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="49" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3824,9 +3722,9 @@
     <row r="988" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="989" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="990" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="991" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="992" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="993" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3868,10 +3766,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -3900,10 +3798,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>

</xml_diff>